<commit_message>
chore: remove unused sheet
</commit_message>
<xml_diff>
--- a/invoice/data/template.xlsx
+++ b/invoice/data/template.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\py-invoice\invoice\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03360D-E066-4FE2-9F97-B2C831633DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D4220-A5AF-443A-A355-F65700BD92BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11625" yWindow="5295" windowWidth="24045" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24855" yWindow="5115" windowWidth="24045" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Yu_Jian" sheetId="1" r:id="rId1"/>
-    <sheet name="Dingyu Xu" sheetId="2" r:id="rId2"/>
+    <sheet name="Dingyu Xu" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,65 +33,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Tax Invoice</t>
   </si>
   <si>
-    <t>Provider Name:</t>
-  </si>
-  <si>
-    <t>Lan Zhang</t>
-  </si>
-  <si>
     <t>ABN:</t>
   </si>
   <si>
-    <t>51628978554</t>
-  </si>
-  <si>
     <t>Email:</t>
   </si>
   <si>
-    <t>lanzhang505@gmail.com</t>
-  </si>
-  <si>
     <t>Mobile:</t>
   </si>
   <si>
-    <t>0452147952</t>
-  </si>
-  <si>
-    <t>Bill to:</t>
-  </si>
-  <si>
-    <t>Well Health Care</t>
-  </si>
-  <si>
-    <t>66628936809</t>
-  </si>
-  <si>
     <t>Address:</t>
   </si>
   <si>
-    <t>Level 3, 2 Brandon Park Drive, Wheelers Hill, VIC, 3150</t>
-  </si>
-  <si>
-    <t>For Providing Service to</t>
-  </si>
-  <si>
-    <t>Yu Jian ( James)</t>
-  </si>
-  <si>
-    <t>41 Rowell Avenue, Camberwell, 3124</t>
-  </si>
-  <si>
     <t>Phone:</t>
   </si>
   <si>
-    <t>0402961871</t>
-  </si>
-  <si>
     <t>Invoice #</t>
   </si>
   <si>
@@ -111,20 +71,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Amount 
-(Ex GST)</t>
-  </si>
-  <si>
-    <t>GST
-Code</t>
-  </si>
-  <si>
-    <t>House Clean</t>
-  </si>
-  <si>
-    <t>Free</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -143,22 +89,10 @@
     <t>Account Number</t>
   </si>
   <si>
-    <t>EFT Payment</t>
-  </si>
-  <si>
-    <t>063109</t>
-  </si>
-  <si>
-    <t>11238355</t>
-  </si>
-  <si>
     <t>Amount (Ex GST)</t>
   </si>
   <si>
     <t>GST Code</t>
-  </si>
-  <si>
-    <t>abcdefg</t>
   </si>
   <si>
     <t>Name:</t>
@@ -171,21 +105,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="d\-mm"/>
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="dd\-mm"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -244,39 +169,28 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -284,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -293,21 +207,13 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="dd\-mm"/>
-      <alignment horizontal="right" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="right" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="d\-mm"/>
       <alignment horizontal="right" vertical="bottom"/>
     </dxf>
   </dxfs>
@@ -324,49 +230,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="E17:F18" totalsRowShown="0">
-  <autoFilter ref="E17:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Invoice #" dataDxfId="3">
-      <calculatedColumnFormula>Table2[[#This Row],[Invoice Date]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Invoice Date" dataDxfId="2">
-      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A20:F23" totalsRowShown="0">
-  <autoFilter ref="A20:F23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Unit"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Rate"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Amount _x000a_(Ex GST)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="GST_x000a_Code"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A27:D28" totalsRowShown="0">
-  <autoFilter ref="A27:D28" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Payment Method"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Account Name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="BSB"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Account Number"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table25" displayName="Table25" ref="E14:F15" totalsRowShown="0">
   <autoFilter ref="E14:F15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
@@ -377,7 +240,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table36" displayName="Table36" ref="A17:F23" totalsRowShown="0">
   <autoFilter ref="A17:F23" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
@@ -392,7 +255,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table17" displayName="Table17" ref="A30:D31" totalsRowShown="0">
   <autoFilter ref="A30:D31" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
@@ -701,249 +564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="8">
-        <f ca="1">Table2[[#This Row],[Invoice Date]]</f>
-        <v>45309</v>
-      </c>
-      <c r="F18" s="12">
-        <f ca="1">TODAY()</f>
-        <v>45309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21">
-        <f>Table3[[#This Row],[Unit]]*Table3[[#This Row],[Rate]]</f>
-        <v>120</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="4">
-        <f>E21+E22</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,161 +582,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="E23" s="4">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="3">
         <f>E18+E19+E20+E21+E22</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>30</v>
+      <c r="A29" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
BREAKING CHANGE: implement first working version
</commit_message>
<xml_diff>
--- a/invoice/data/template.xlsx
+++ b/invoice/data/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\py-invoice\invoice\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D4220-A5AF-443A-A355-F65700BD92BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F686FE99-C5C1-4A87-ABCD-E496D96900A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24855" yWindow="5115" windowWidth="24045" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29070" yWindow="3570" windowWidth="24030" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dingyu Xu" sheetId="2" r:id="rId1"/>
@@ -105,9 +105,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd\-mm"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="dd\-mm"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -171,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -186,10 +187,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -202,6 +203,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -209,11 +211,11 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right" vertical="bottom"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd\-mm"/>
+      <numFmt numFmtId="164" formatCode="dd\-mm"/>
       <alignment horizontal="right" vertical="bottom"/>
     </dxf>
   </dxfs>
@@ -568,7 +570,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +712,7 @@
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="E23" s="3">
+      <c r="E23" s="14">
         <f>E18+E19+E20+E21+E22</f>
         <v>0</v>
       </c>

</xml_diff>